<commit_message>
Added Comparator logic external excel file with required utilities
</commit_message>
<xml_diff>
--- a/resources/templates/TemperatureCalculationFolder/TemperatureCalculation.xlsx
+++ b/resources/templates/TemperatureCalculationFolder/TemperatureCalculation.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhi1\MyHomeStudy(Automation Complete)\WorkspaceCodingAssignment\CodingAssignmentProject\CodingAssignmentProject\resources\templates\TemperatureCalculationFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19E6313-5612-4DAF-AF2D-00B6489CEB83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D1DFCD-60C5-4841-85FA-10C74C0BC3C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -61,6 +61,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -412,15 +413,15 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.08984375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.1796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.7421875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.08984375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -441,32 +442,32 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>30</v>
+      <c r="B2" s="1" t="n">
+        <v>22.0</v>
       </c>
       <c r="C2" s="1">
         <f>B2-B5</f>
-        <v>-2.9450000000000003</v>
+        <v>-1.7899999618529989</v>
       </c>
       <c r="D2" s="1">
         <f>C2^2</f>
-        <v>8.6730250000000009</v>
+        <v>3.2040998634337376</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>35.89</v>
+      <c r="B3" s="1" t="n">
+        <v>25.579999923706055</v>
       </c>
       <c r="C3" s="1">
         <f>B3-B5</f>
-        <v>2.9450000000000003</v>
+        <v>1.7899999618530025</v>
       </c>
       <c r="D3" s="1">
         <f>C3^2</f>
-        <v>8.6730250000000009</v>
+        <v>3.2040998634337505</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -481,14 +482,14 @@
       </c>
       <c r="B5" s="1">
         <f>AVERAGE(B2:B3)</f>
-        <v>32.945</v>
+        <v>23.789999961852999</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1">
         <f>D2+D3</f>
-        <v>17.346050000000002</v>
+        <v>6.4081997268674886</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -499,7 +500,7 @@
       </c>
       <c r="D6" s="1">
         <f>D5/2</f>
-        <v>8.6730250000000009</v>
+        <v>3.2040998634337443</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added Listeners and Extent Reporting
</commit_message>
<xml_diff>
--- a/resources/templates/TemperatureCalculationFolder/TemperatureCalculation.xlsx
+++ b/resources/templates/TemperatureCalculationFolder/TemperatureCalculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhi1\MyHomeStudy(Automation Complete)\WorkspaceCodingAssignment\CodingAssignmentProject\CodingAssignmentProject\resources\templates\TemperatureCalculationFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D1DFCD-60C5-4841-85FA-10C74C0BC3C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57083A0-DFA1-4671-B1A5-F50F5E95EBC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,11 +447,11 @@
       </c>
       <c r="C2" s="1">
         <f>B2-B5</f>
-        <v>-1.7899999618529989</v>
+        <v>-1.0799999237060476</v>
       </c>
       <c r="D2" s="1">
         <f>C2^2</f>
-        <v>3.2040998634337376</v>
+        <v>1.1663998352050686</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -459,15 +459,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>25.579999923706055</v>
+        <v>22.420000076293945</v>
       </c>
       <c r="C3" s="1">
         <f>B3-B5</f>
-        <v>1.7899999618530025</v>
+        <v>1.0799999237060511</v>
       </c>
       <c r="D3" s="1">
         <f>C3^2</f>
-        <v>3.2040998634337505</v>
+        <v>1.1663998352050762</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -482,14 +482,14 @@
       </c>
       <c r="B5" s="1">
         <f>AVERAGE(B2:B3)</f>
-        <v>23.789999961852999</v>
+        <v>23.079999923706048</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1">
         <f>D2+D3</f>
-        <v>6.4081997268674886</v>
+        <v>2.3327996704101448</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -500,7 +500,7 @@
       </c>
       <c r="D6" s="1">
         <f>D5/2</f>
-        <v>3.2040998634337443</v>
+        <v>1.1663998352050724</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -511,7 +511,7 @@
       </c>
       <c r="D7" s="1" t="b">
         <f>IF(D6&lt;3, TRUE, FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>